<commit_message>
Custom filename + multiple objects in single dat
Create a column called filename and optionally set a custom dat name
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>Shoes 1950</t>
   </si>
@@ -135,15 +135,9 @@
     <t>The tool does not check the validity of the dat, it just takes whatever is in the first row at that column and write it in the dat followed by = and the value of the cell.</t>
   </si>
   <si>
-    <t>Also worth noting that the order you put things in here is (or should be) the orderof the exported dat.</t>
-  </si>
-  <si>
     <t>Anyway, using the name parameter or a friendly name is the best option to take advantage of Excel's feature of freezing the first row and column as you scroll.</t>
   </si>
   <si>
-    <t>In this sheet we decided to not have friendly names for the objects and put in column A the [name] parameter directly.</t>
-  </si>
-  <si>
     <t>You can put any paramater in column A, as explained in the first sheet as long as there's any data in column A that row becomes a dat.</t>
   </si>
   <si>
@@ -169,13 +163,177 @@
   </si>
   <si>
     <t>Functions are allowed as long as they return the above types (see C3, C4, D3, D4)</t>
+  </si>
+  <si>
+    <t>Also worth noting that the order you put things in here is (or should be) the order of the exported dat.</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>wood_containers</t>
+  </si>
+  <si>
+    <t>wood_c1_40</t>
+  </si>
+  <si>
+    <t>wood_c2_10</t>
+  </si>
+  <si>
+    <t>Volvo_750</t>
+  </si>
+  <si>
+    <t>volvo_750hp_2015</t>
+  </si>
+  <si>
+    <r>
+      <t>In this sheet we decided to not have friendly names for the objects and put in column A the '</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> parameter directly.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>By  default the tool creates a dat with the same name as the '</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">name' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parameter, but if you specify something under '</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filename'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, this will be the name of the dat file.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This sheet also has the only special parameter key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>wood_c3_30</t>
+  </si>
+  <si>
+    <t>Setting the filename is also the way to write multiple objects into a single dat file</t>
+  </si>
+  <si>
+    <t>As long as multiple objects have the same filename AND are in direct succession (one right after the other without interval) they will all be in the same dat</t>
+  </si>
+  <si>
+    <t>The text at E7 tells clearly that writing a filename previously defined would destroy the data you had.</t>
+  </si>
+  <si>
+    <t>Tip: Excel and Calc have buttons to add an empty row anywhere you wish to let you add more objects into a single dat</t>
+  </si>
+  <si>
+    <t>&lt; This is wrong, it will overwrite the previous wood_container created by rows 3 with the contents of rows 5-7</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt; The dat file name will be taken from '</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +343,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -647,17 +813,17 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -667,17 +833,17 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -688,7 +854,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -760,12 +926,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,6 +947,31 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -791,21 +982,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -815,61 +1007,122 @@
       <c r="C1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="C3">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>